<commit_message>
#2651 4º Checklist da Qualidade
Checkilist da Qualidade referente à construção 4

Correção da planilha do 3º Checklist
</commit_message>
<xml_diff>
--- a/Doc-DD-UFG/Qualidade/Gerência/checklist_qualidade_GCO-1.1.0_SDD-UFG201511251720.xlsx
+++ b/Doc-DD-UFG/Qualidade/Gerência/checklist_qualidade_GCO-1.1.0_SDD-UFG201511251720.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marla Aragão\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marla Aragão\Documents\GitHub\sdd-ufg\Doc-DD-UFG\Qualidade\Gerência\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -78,16 +78,16 @@
     <t>Evidencia 2</t>
   </si>
   <si>
-    <t>Não</t>
-  </si>
-  <si>
     <t>Os papeis referentes a este projeto foram identificados no plano e estão listados em alguma tarefa do cronograma?</t>
   </si>
   <si>
     <t xml:space="preserve">Toda a equipe se comprometeu e aprovou o plano de configuração? </t>
   </si>
   <si>
-    <t>Não há evidências que mostrem que auditorias foram efetuadas na baseline.</t>
+    <t>Não há prazo para auditoria especificado no Plano de Projeto, impossibilitando determinar se já deveria ter ocorrido auditoria ou não para a baseline criada.</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -658,12 +658,12 @@
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -742,7 +742,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
@@ -762,7 +762,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>6</v>

</xml_diff>